<commit_message>
Implemented Bulk Manufacturers Upload
</commit_message>
<xml_diff>
--- a/client/public/BulkUploadManufacturers.xlsx
+++ b/client/public/BulkUploadManufacturers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolimitmide/Desktop/tyu/client/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6cd9fd63bb338099/Desktop/PIM/client/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{425BB964-9278-974A-B4A9-CA3CB3F77392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{425BB964-9278-974A-B4A9-CA3CB3F77392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{961E3A8C-328C-4CED-96A3-E7D645D4E71A}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{B964F389-F697-5240-B4F3-E79D88D6B699}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{B964F389-F697-5240-B4F3-E79D88D6B699}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Manufacturer</t>
   </si>
   <si>
     <t>Brands</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>testgg</t>
+  </si>
+  <si>
+    <t>testggr</t>
+  </si>
+  <si>
+    <t>testggt</t>
+  </si>
+  <si>
+    <t>testggy</t>
+  </si>
+  <si>
+    <t>testggu</t>
   </si>
 </sst>
 </file>
@@ -413,20 +443,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C49BBEC-4CEE-7A48-A279-5C1557DE08FA}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>